<commit_message>
module 2,3 ok (3 còn xuất file)
</commit_message>
<xml_diff>
--- a/docs/TemplateOffices/xlxs/sinhvien.xlsx
+++ b/docs/TemplateOffices/xlxs/sinhvien.xlsx
@@ -25,12 +25,6 @@
     <t>tenSinhVien</t>
   </si>
   <si>
-    <t>KhoaHoc</t>
-  </si>
-  <si>
-    <t>NganhHoc</t>
-  </si>
-  <si>
     <t>Vũ Minh Tuấn</t>
   </si>
   <si>
@@ -185,6 +179,12 @@
   </si>
   <si>
     <t>httt</t>
+  </si>
+  <si>
+    <t>KhoaHocKh</t>
+  </si>
+  <si>
+    <t>NganhHocKh</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,10 +591,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -603,16 +603,16 @@
         <v>14020521</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -621,17 +621,17 @@
         <v>14020441</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>CONCATENATE(A3,"@vnu.edu.vn")</f>
+        <f t="shared" ref="C3:C17" si="0">CONCATENATE(A3,"@vnu.edu.vn")</f>
         <v>14020441@vnu.edu.vn</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -640,17 +640,17 @@
         <v>14020450</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>CONCATENATE(A4,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020450@vnu.edu.vn</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -659,17 +659,17 @@
         <v>14020451</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>CONCATENATE(A5,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020451@vnu.edu.vn</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -678,17 +678,17 @@
         <v>14020452</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>CONCATENATE(A6,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020452@vnu.edu.vn</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -697,17 +697,17 @@
         <v>14020465</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>CONCATENATE(A7,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020465@vnu.edu.vn</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -716,17 +716,17 @@
         <v>14020470</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>CONCATENATE(A8,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020470@vnu.edu.vn</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -735,17 +735,17 @@
         <v>14020477</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>CONCATENATE(A9,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020477@vnu.edu.vn</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -754,17 +754,17 @@
         <v>14020485</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f>CONCATENATE(A10,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020485@vnu.edu.vn</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -773,17 +773,17 @@
         <v>14020488</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>CONCATENATE(A11,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020488@vnu.edu.vn</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -792,17 +792,17 @@
         <v>14020494</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f>CONCATENATE(A12,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020494@vnu.edu.vn</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -811,17 +811,17 @@
         <v>14020502</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f>CONCATENATE(A13,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020502@vnu.edu.vn</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -830,17 +830,17 @@
         <v>14020503</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f>CONCATENATE(A14,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020503@vnu.edu.vn</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -849,17 +849,17 @@
         <v>14020513</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f>CONCATENATE(A15,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020513@vnu.edu.vn</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -868,17 +868,17 @@
         <v>14020515</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="str">
-        <f>CONCATENATE(A16,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020515@vnu.edu.vn</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -887,17 +887,17 @@
         <v>14020520</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="str">
-        <f>CONCATENATE(A17,"@vnu.edu.vn")</f>
+        <f t="shared" si="0"/>
         <v>14020520@vnu.edu.vn</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -906,17 +906,17 @@
         <v>14020578</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" ref="C18:C47" si="0">CONCATENATE(A18,"@vnu.edu.vn")</f>
+        <f t="shared" ref="C18:C47" si="1">CONCATENATE(A18,"@vnu.edu.vn")</f>
         <v>14020578@vnu.edu.vn</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -925,17 +925,17 @@
         <v>14020061</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020061@vnu.edu.vn</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,17 +943,17 @@
         <v>14020069</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020069@vnu.edu.vn</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,17 +961,17 @@
         <v>13020526</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020526@vnu.edu.vn</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,17 +979,17 @@
         <v>14020088</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020088@vnu.edu.vn</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -997,17 +997,17 @@
         <v>14020092</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020092@vnu.edu.vn</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,17 +1015,17 @@
         <v>13020099</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020099@vnu.edu.vn</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1033,17 +1033,17 @@
         <v>14020582</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020582@vnu.edu.vn</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,17 +1051,17 @@
         <v>13020113</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020113@vnu.edu.vn</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,17 +1069,17 @@
         <v>13020540</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020540@vnu.edu.vn</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,17 +1087,17 @@
         <v>14020585</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020585@vnu.edu.vn</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,17 +1105,17 @@
         <v>14020146</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020146@vnu.edu.vn</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1123,17 +1123,17 @@
         <v>12020125</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12020125@vnu.edu.vn</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1141,17 +1141,17 @@
         <v>14020156</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020156@vnu.edu.vn</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,17 +1159,17 @@
         <v>14020161</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020161@vnu.edu.vn</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,17 +1177,17 @@
         <v>14020162</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020162@vnu.edu.vn</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1195,17 +1195,17 @@
         <v>14020165</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020165@vnu.edu.vn</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1213,17 +1213,17 @@
         <v>13020159</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020159@vnu.edu.vn</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1231,17 +1231,17 @@
         <v>11020118</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11020118@vnu.edu.vn</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,17 +1249,17 @@
         <v>14020185</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020185@vnu.edu.vn</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1267,17 +1267,17 @@
         <v>14020188</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020188@vnu.edu.vn</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,17 +1285,17 @@
         <v>13020169</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13020169@vnu.edu.vn</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,17 +1303,17 @@
         <v>14020217</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020217@vnu.edu.vn</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1321,17 +1321,17 @@
         <v>14020219</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C41" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020219@vnu.edu.vn</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,17 +1339,17 @@
         <v>14020213</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020213@vnu.edu.vn</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,17 +1357,17 @@
         <v>14020239</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C43" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020239@vnu.edu.vn</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,17 +1375,17 @@
         <v>14020246</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020246@vnu.edu.vn</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1393,17 +1393,17 @@
         <v>14020248</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C45" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020248@vnu.edu.vn</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1411,17 +1411,17 @@
         <v>14020249</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C46" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14020249@vnu.edu.vn</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,17 +1429,17 @@
         <v>12020215</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12020215@vnu.edu.vn</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>